<commit_message>
تعديل تلقائي في شيت Card24 by admin at 2025-11-29 18:45:23
</commit_message>
<xml_diff>
--- a/elquds.xlsx
+++ b/elquds.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,11 +534,6 @@
           <t>Servised by</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Serviced by</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -561,26 +556,61 @@
           <t>.1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
           <t>تم التشغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O2" t="inlineStr">
         <is>
           <t>م.صيام</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -598,19 +628,66 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -628,19 +705,66 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -658,19 +782,66 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -693,7 +864,11 @@
           <t>632</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -714,17 +889,36 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -747,7 +941,11 @@
           <t>870</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -758,19 +956,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>6\10\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -788,19 +1013,66 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -818,19 +1090,66 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -848,19 +1167,66 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -878,19 +1244,66 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -908,19 +1321,83 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5844,7 +6321,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5913,254 +6390,86 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Serviced by</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>150</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>151</v>
+      </c>
+      <c r="C3" t="n">
+        <v>300</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>21\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>301</v>
+      </c>
+      <c r="C4" t="n">
+        <v>450</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>451</v>
+      </c>
+      <c r="C5" t="n">
+        <v>550</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6176,165 +6485,73 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>19\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>573</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>551</v>
+      </c>
+      <c r="C6" t="n">
+        <v>700</v>
+      </c>
+      <c r="D6" t="n">
+        <v>573</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>8\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>729</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>701</v>
+      </c>
+      <c r="C7" t="n">
+        <v>850</v>
+      </c>
+      <c r="D7" t="n">
+        <v>729</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6345,448 +6562,120 @@
           <t>7\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>931</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>851</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>869</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>✔</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">م.محمد عبدالله </t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>تم سن الفلاتس لاول مره بعد التغير</t>
+          <t>30\9\2025</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>869</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>30\9\2025</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1150</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1151</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1301</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1450</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1451</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8030,7 +7919,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>event</t>
+          <t>Event</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">

</xml_diff>

<commit_message>
إضافة حدث جديد في Card24 by admin at 2025-11-30 18:59:27
</commit_message>
<xml_diff>
--- a/elquds.xlsx
+++ b/elquds.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,6 +534,11 @@
           <t>Servised by</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -611,6 +616,11 @@
           <t>م.صيام</t>
         </is>
       </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -688,6 +698,11 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -765,6 +780,11 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -842,6 +862,11 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -919,6 +944,11 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -996,6 +1026,11 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1073,6 +1108,11 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1150,6 +1190,11 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1227,6 +1272,11 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1304,6 +1354,11 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1381,23 +1436,131 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>12\11\2024</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>خلل ف عيار</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>اعاده عيار</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>11\2\2025</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>وقت زيت</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>تم تغير زيت</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2627,7 +2790,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2696,16 +2859,37 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -2716,19 +2900,30 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="n">
-        <v>159</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -2750,16 +2945,25 @@
           <t>15\7\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -2770,16 +2974,25 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
@@ -2806,19 +3019,30 @@
           <t>1\3\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>591</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>591</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -2836,19 +3060,30 @@
           <t>19\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>758</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>758</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
@@ -2874,70 +3109,115 @@
           <t>23\7\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>895</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>999</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>13\10\2025</t>
-        </is>
-      </c>
+          <t>30/11/2025</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>م.محمد عبدالله ،خبير.ارول</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>895</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>13\10\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -2948,16 +3228,25 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -2968,16 +3257,25 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -2988,6 +3286,38 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3000,7 +3330,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3069,16 +3399,42 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by.1</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -3089,16 +3445,26 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
@@ -3121,16 +3487,26 @@
           <t>16\7\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -3141,16 +3517,26 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
@@ -3177,19 +3563,31 @@
           <t>8\3\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>595</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>595</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -3207,19 +3605,31 @@
           <t>17\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>764</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>764</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
@@ -3245,19 +3655,31 @@
           <t>21\7\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>899</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>899</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
@@ -3279,38 +3701,78 @@
           <t>9\10\2025</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1049</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>29/11/2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>م.محمد عبدالله ،ف.محمود ايهاب</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1039</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
@@ -3318,17 +3780,43 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>22/11/2025</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>انكسار حساس icfd</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">تم استبدال </t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>م.اشرف كهرباء ،ف. سعيد السيد</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -3339,16 +3827,26 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -3359,6 +3857,40 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3371,7 +3903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3440,16 +3972,37 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -3460,16 +4013,25 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
@@ -3492,16 +4054,25 @@
           <t>20\7\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -3512,16 +4083,25 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
@@ -3552,19 +4132,30 @@
           <t>6\3\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>584</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>584</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -3582,19 +4173,30 @@
           <t>14\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>753</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>753</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
@@ -3620,70 +4222,115 @@
           <t>20\7\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>887</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>967</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>8\10\2025</t>
+          <t>27/11/2025</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>م.محمد عبدالله ،ف.مصطفي</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>887</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>8\10\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -3694,16 +4341,25 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -3714,16 +4370,25 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -3734,6 +4399,38 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3746,7 +4443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3815,16 +4512,37 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -3835,19 +4553,30 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="n">
-        <v>159</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -3869,16 +4598,25 @@
           <t>21\7\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -3889,16 +4627,25 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
@@ -3929,19 +4676,30 @@
           <t>28\1\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>578</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>578</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -3959,19 +4717,30 @@
           <t>13\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>749</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>749</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
@@ -3993,19 +4762,30 @@
           <t>19\7\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>880</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>880</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
@@ -4027,36 +4807,70 @@
           <t>5\10\2025</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1013</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>26/11/2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>م محمد عبدالله ،ف.محمود ايهاب</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -4067,16 +4881,25 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -4087,16 +4910,25 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -4107,6 +4939,9 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4119,7 +4954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4188,16 +5023,37 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -4208,16 +5064,25 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
@@ -4240,16 +5105,25 @@
           <t>1\7\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -4260,16 +5134,25 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
@@ -4300,19 +5183,30 @@
           <t>20\1\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>573</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>573</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -4330,19 +5224,30 @@
           <t>12\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>742</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>742</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
@@ -4364,70 +5269,115 @@
           <t>17\7\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>873</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>995</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>4\10\2025</t>
+          <t>25/11/2025</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>م.محمد عبدالله ،ف.محمود ايهاب</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>873</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>4\10\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -4438,16 +5388,25 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -4458,16 +5417,25 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -4478,6 +5446,38 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4917,7 +5917,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4986,16 +5986,37 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -5006,19 +6027,30 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="n">
-        <v>177</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>177</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -5040,16 +6072,25 @@
           <t>20\7\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -5060,16 +6101,25 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
@@ -5096,19 +6146,30 @@
           <t>5\3\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>579</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>579</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -5126,19 +6187,30 @@
           <t>9\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>739</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>739</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
@@ -5164,70 +6236,119 @@
           <t>9\7\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>880</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>944.7</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>1\10\2025</t>
+          <t>8/11/2025</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>تم السن اول مره بعد تغيير</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>م.محمد عبدالله+ف.محمود ايهاب</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>880</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>1\10\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -5238,16 +6359,25 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -5258,16 +6388,25 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -5278,6 +6417,38 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5948,7 +7119,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6017,16 +7188,37 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -6037,19 +7229,30 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="n">
-        <v>177</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>177</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -6071,16 +7274,25 @@
           <t>21\7\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -6091,16 +7303,25 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
@@ -6131,19 +7352,30 @@
           <t>27\1\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>566</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>566</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -6161,19 +7393,30 @@
           <t>10\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>737</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>737</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
@@ -6195,70 +7438,119 @@
           <t>16\7\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>851</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>953</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>22\9\2025</t>
+          <t>23/11/2025</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>تم سن الفلاتس</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">م.محمد عبدالله </t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>22\9\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -6269,16 +7561,25 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -6289,16 +7590,25 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -6309,6 +7619,38 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6321,7 +7663,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6390,16 +7732,32 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -6410,16 +7768,24 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
@@ -6438,16 +7804,24 @@
           <t>21\7\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -6458,16 +7832,24 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
@@ -6498,19 +7880,29 @@
           <t>19\1\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>573</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>573</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -6528,19 +7920,29 @@
           <t>8\4\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>729</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>729</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
@@ -6562,70 +7964,116 @@
           <t>7\7\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>869</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>931</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>30\9\2025</t>
+          <t>6/11/2025</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">م.محمد عبدالله </t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>تم سن الفلاتس لاول مره بعد التغير</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>869</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>30\9\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -6636,16 +8084,24 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -6656,16 +8112,24 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -6676,6 +8140,36 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7919,7 +9413,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Event</t>
+          <t>event</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -9034,7 +10528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9505,6 +10999,39 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>12\11\2024</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>خلل ف عيار</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>اعاده عيار</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card23 by admin at 2025-11-30 19:17:03
</commit_message>
<xml_diff>
--- a/elquds.xlsx
+++ b/elquds.xlsx
@@ -561,66 +561,26 @@
           <t>.1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
           <t>تم التشغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>م.صيام</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -638,71 +598,19 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -720,71 +628,19 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -802,71 +658,19 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -889,11 +693,7 @@
           <t>632</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -914,41 +714,17 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -971,11 +747,7 @@
           <t>870</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -986,51 +758,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>6\10\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1048,71 +788,19 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1130,71 +818,19 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1212,71 +848,19 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1294,71 +878,19 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1376,71 +908,19 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1448,56 +928,16 @@
           <t>24</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
           <t>12\11\2024</t>
@@ -1513,16 +953,8 @@
           <t>اعاده عيار</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -6461,7 +5893,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6530,38 +5962,96 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Servised by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6572,48 +6062,122 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>6\8\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6629,64 +6193,122 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>23\1\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>641</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>641</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>15\5\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>836</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>836</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6697,115 +6319,378 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>4\9\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2\2\2025</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>م.عبدالله</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card1 by admin at 2025-11-30 19:18:55
</commit_message>
<xml_diff>
--- a/elquds.xlsx
+++ b/elquds.xlsx
@@ -5984,51 +5984,15 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -6047,11 +6011,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6062,31 +6022,11 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>6\8\2024</t>
@@ -6110,51 +6050,15 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -6173,11 +6077,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6193,26 +6093,14 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>23\1\2025</t>
@@ -6241,41 +6129,17 @@
           <t>641</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>15\5\2025</t>
@@ -6304,11 +6168,7 @@
           <t>836</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6319,26 +6179,10 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>4\9\2025</t>
@@ -6362,51 +6206,15 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -6425,51 +6233,15 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -6488,51 +6260,15 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -6551,51 +6287,15 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -6614,51 +6314,15 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
@@ -9227,7 +8891,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9328,14 +8992,46 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>1/2/2024</t>
@@ -9346,7 +9042,11 @@
           <t>تم تشغيل الماكينه اول مره</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O2" t="inlineStr">
         <is>
           <t>زكريا</t>
@@ -9384,19 +9084,51 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>15\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -9414,14 +9146,46 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>11\8\2024</t>
@@ -9459,14 +9223,46 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>29\9\2024</t>
@@ -9504,20 +9300,56 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>22\12\2024</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="N6" t="inlineStr">
         <is>
           <t>صيانه نصف سنويه</t>
@@ -9545,18 +9377,66 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -9574,7 +9454,11 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -9590,22 +9474,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>29\1\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -9628,29 +9536,61 @@
           <t>565</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L9" t="inlineStr">
         <is>
           <t>5\4\2025</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -9673,16 +9613,36 @@
           <t>724</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
           <t>✔</t>
@@ -9693,9 +9653,21 @@
           <t>5\7\2025</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -9718,25 +9690,61 @@
           <t>859</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L11" t="inlineStr">
         <is>
           <t>24\9\2025</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -9754,18 +9762,66 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -9783,18 +9839,66 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -9812,18 +9916,66 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -9841,18 +9993,107 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2\2\2025</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>خلل ف عيار</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>تم اعاده عيار</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>م.عبدالله</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card2 by admin at 2025-11-30 19:22:37
</commit_message>
<xml_diff>
--- a/elquds.xlsx
+++ b/elquds.xlsx
@@ -8992,1221 +8992,6 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1/2/2024</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>تم تشغيل الماكينه اول مره</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>زكريا</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>159</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>15\7\2024</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>11\8\2024</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>4300 ساعه تشغيل</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>تم التشحيم شحم Ep3</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>حسام</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>29\9\2024</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>زياره توكيل</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>اعاده عيار ماكينه</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>م.صيام</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>22\12\2024</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>صيانه نصف سنويه</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>تيم العمل</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>29\1\2025</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>565</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>5\4\2025</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>724</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>5\7\2025</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>859</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>24\9\2025</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>2\2\2025</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>خلل ف عيار</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>تم اعاده عيار</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>م.عبدالله</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>card</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Min_Tones</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Max_Tones</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Tones</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Revolving flats(x)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>1.carding elemnt(o)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>licker_in carding element(o)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Doffer carding element(o)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>cylinder(X)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>doffer(X)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Revolving flats(o)</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Correction</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Serviced by</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -10215,23 +9000,27 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1/2/2024</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>تم الشتغيل</t>
+          <t>تم تشغيل الماكينه اول مره</t>
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
-          <t>A.Elshenawy</t>
+          <t>زكريا</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -10244,7 +9033,11 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10262,7 +9055,7 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>16\7\2024</t>
+          <t>15\7\2024</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
@@ -10272,62 +9065,62 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>27\2\2025</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+          <t>11\8\2024</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>4300 ساعه تشغيل</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>تم التشحيم شحم Ep3</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>حسام</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -10338,93 +9131,93 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>29\9\2024</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>زياره توكيل</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>اعاده عيار ماكينه</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>م.صيام</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>559</t>
-        </is>
-      </c>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>7\4\2025</t>
+          <t>22\12\2024</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>صيانه نصف سنويه</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>تيم العمل</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>727</t>
-        </is>
-      </c>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>6\7\2025</t>
-        </is>
-      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -10432,25 +9225,25 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>860</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10462,96 +9255,108 @@
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>28\9\2025</t>
+          <t>29\1\2025</t>
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>م.محمد عبدالله</t>
-        </is>
-      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>700</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>918</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+          <t>565</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>1\11\2025</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">تم سن فلاتس وعياره </t>
-        </is>
-      </c>
+          <t>5\4\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">م.محمد عبدالله </t>
-        </is>
-      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>724</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>5\7\2025</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
@@ -10559,28 +9364,40 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>859</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>24\9\2025</t>
+        </is>
+      </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
@@ -10588,17 +9405,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1301</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1450</t>
+          <t>1150</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -10617,17 +9434,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1451</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>1300</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -10642,6 +9459,1166 @@
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2\2\2025</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>خلل ف عيار</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>تم اعاده عيار</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>م.عبدالله</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>card</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Min_Tones</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Max_Tones</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tones</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Revolving flats(x)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>1.carding elemnt(o)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>licker_in carding element(o)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Doffer carding element(o)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>cylinder(X)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>doffer(X)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Revolving flats(o)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>تم الشتغيل</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>A.Elshenawy</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>16\7\2024</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>27\2\2025</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>559</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>7\4\2025</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>727</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>6\7\2025</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>860</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>28\9\2025</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>م.محمد عبدالله</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>918</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>1\11\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">تم سن فلاتس وعياره </t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">م.محمد عبدالله </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2\2\2025</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>خلل ف عيار</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>تم اعاده عيار</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>م.عبدالله</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card2 by admin at 2025-11-30 19:26:23
</commit_message>
<xml_diff>
--- a/elquds.xlsx
+++ b/elquds.xlsx
@@ -9570,7 +9570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10585,20 +10585,56 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>99</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L14" t="inlineStr">
         <is>
           <t>2\2\2025</t>
@@ -10617,6 +10653,47 @@
       <c r="O14" t="inlineStr">
         <is>
           <t>م.عبدالله</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>2\11\2025</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>قطع سير 1270</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>تغير سير 1270</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>حسام</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card1 by admin at 2025-11-30 19:27:50
</commit_message>
<xml_diff>
--- a/elquds.xlsx
+++ b/elquds.xlsx
@@ -8891,7 +8891,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8992,6 +8992,1298 @@
           <t>150</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1/2/2024</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>تم تشغيل الماكينه اول مره</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>زكريا</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>15\7\2024</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>11\8\2024</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>4300 ساعه تشغيل</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>تم التشحيم شحم Ep3</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>حسام</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>29\9\2024</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>زياره توكيل</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>اعاده عيار ماكينه</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>م.صيام</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>22\12\2024</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>صيانه نصف سنويه</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>تيم العمل</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>29\1\2025</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>565</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>5\4\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>724</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>5\7\2025</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>859</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>24\9\2025</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2\2\2025</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>خلل ف عيار</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>تم اعاده عيار</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>م.عبدالله</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2\11\2025</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>قطع سير 1270</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>تغير سير 1270</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>حسام</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>card</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Min_Tones</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Max_Tones</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tones</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Revolving flats(x)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>1.carding elemnt(o)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>licker_in carding element(o)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Doffer carding element(o)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>cylinder(X)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>doffer(X)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Revolving flats(o)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -9000,27 +10292,23 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1/2/2024</t>
-        </is>
-      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>تم تشغيل الماكينه اول مره</t>
+          <t>تم الشتغيل</t>
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
-          <t>زكريا</t>
+          <t>A.Elshenawy</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -9033,11 +10321,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>159</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -9055,7 +10339,7 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>15\7\2024</t>
+          <t>16\7\2024</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
@@ -9065,62 +10349,62 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>450</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>11\8\2024</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>4300 ساعه تشغيل</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>تم التشحيم شحم Ep3</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>حسام</t>
-        </is>
-      </c>
+          <t>27\2\2025</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>550</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -9131,93 +10415,93 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>29\9\2024</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>زياره توكيل</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>اعاده عيار ماكينه</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>م.صيام</t>
-        </is>
-      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>559</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>22\12\2024</t>
+          <t>7\4\2025</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>صيانه نصف سنويه</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>تيم العمل</t>
-        </is>
-      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>727</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>6\7\2025</t>
+        </is>
+      </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -9225,25 +10509,25 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>860</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -9255,108 +10539,96 @@
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>29\1\2025</t>
+          <t>28\9\2025</t>
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>م.محمد عبدالله</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>565</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>918</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>5\4\2025</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr"/>
+          <t>1\11\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">تم سن فلاتس وعياره </t>
+        </is>
+      </c>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">م.محمد عبدالله </t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>724</t>
-        </is>
-      </c>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>5\7\2025</t>
-        </is>
-      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
@@ -9364,40 +10636,28 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>859</t>
-        </is>
-      </c>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>24\9\2025</t>
-        </is>
-      </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
@@ -9405,17 +10665,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>1301</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>1450</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -9434,17 +10694,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>1451</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -9463,20 +10723,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
@@ -9484,1216 +10740,24 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>2\2\2025</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>خلل ف عيار</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>تم اعاده عيار</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>م.عبدالله</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>card</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Min_Tones</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Max_Tones</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Tones</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Revolving flats(x)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>1.carding elemnt(o)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>licker_in carding element(o)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Doffer carding element(o)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>cylinder(X)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>doffer(X)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Revolving flats(o)</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Correction</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Serviced by</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>تم الشتغيل</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>A.Elshenawy</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>16\7\2024</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>27\2\2025</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>559</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>7\4\2025</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>727</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>6\7\2025</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>860</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>28\9\2025</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>م.محمد عبدالله</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>918</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>1\11\2025</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">تم سن فلاتس وعياره </t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">م.محمد عبدالله </t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>2\2\2025</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>خلل ف عيار</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>تم اعاده عيار</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>م.عبدالله</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>990</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>2\11\2025</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>قطع سير 1270</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>تغير سير 1270</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>حسام</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card2 by admin at 2025-12-01 06:14:50
</commit_message>
<xml_diff>
--- a/elquds.xlsx
+++ b/elquds.xlsx
@@ -8992,1298 +8992,6 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1/2/2024</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>تم تشغيل الماكينه اول مره</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>زكريا</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>159</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>15\7\2024</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>11\8\2024</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>4300 ساعه تشغيل</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>تم التشحيم شحم Ep3</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>حسام</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>29\9\2024</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>زياره توكيل</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>اعاده عيار ماكينه</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>م.صيام</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>22\12\2024</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>صيانه نصف سنويه</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>تيم العمل</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>29\1\2025</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>565</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>5\4\2025</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>724</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>5\7\2025</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>859</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>24\9\2025</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>2\2\2025</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>خلل ف عيار</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>تم اعاده عيار</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>م.عبدالله</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>990</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>2\11\2025</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>قطع سير 1270</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>تغير سير 1270</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>حسام</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>card</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Min_Tones</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Max_Tones</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Tones</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Revolving flats(x)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>1.carding elemnt(o)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>licker_in carding element(o)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Doffer carding element(o)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>cylinder(X)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>doffer(X)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Revolving flats(o)</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Correction</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Serviced by</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -10292,23 +9000,27 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1/2/2024</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>تم الشتغيل</t>
+          <t>تم تشغيل الماكينه اول مره</t>
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
-          <t>A.Elshenawy</t>
+          <t>زكريا</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -10321,7 +9033,11 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10339,7 +9055,7 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>16\7\2024</t>
+          <t>15\7\2024</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
@@ -10349,62 +9065,62 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>27\2\2025</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+          <t>11\8\2024</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>4300 ساعه تشغيل</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>تم التشحيم شحم Ep3</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>حسام</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -10415,93 +9131,93 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>29\9\2024</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>زياره توكيل</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>اعاده عيار ماكينه</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>م.صيام</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>559</t>
-        </is>
-      </c>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>7\4\2025</t>
+          <t>22\12\2024</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>صيانه نصف سنويه</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>تيم العمل</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>727</t>
-        </is>
-      </c>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>6\7\2025</t>
-        </is>
-      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -10509,25 +9225,25 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>860</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10539,96 +9255,108 @@
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>28\9\2025</t>
+          <t>29\1\2025</t>
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>م.محمد عبدالله</t>
-        </is>
-      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>700</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>918</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+          <t>565</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>1\11\2025</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">تم سن فلاتس وعياره </t>
-        </is>
-      </c>
+          <t>5\4\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">م.محمد عبدالله </t>
-        </is>
-      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>724</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>5\7\2025</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
@@ -10636,28 +9364,40 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>859</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>24\9\2025</t>
+        </is>
+      </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
@@ -10665,17 +9405,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1301</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1450</t>
+          <t>1150</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -10694,17 +9434,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1451</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>1300</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -10723,16 +9463,20 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
@@ -10740,6 +9484,1198 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2\2\2025</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>خلل ف عيار</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>تم اعاده عيار</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>م.عبدالله</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2\11\2025</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>قطع سير 1270</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>تغير سير 1270</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>حسام</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>card</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Min_Tones</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Max_Tones</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tones</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Revolving flats(x)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>1.carding elemnt(o)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>licker_in carding element(o)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Doffer carding element(o)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>cylinder(X)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>doffer(X)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Revolving flats(o)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>تم الشتغيل</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>A.Elshenawy</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>16\7\2024</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>27\2\2025</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>559</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>7\4\2025</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>727</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>6\7\2025</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>860</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>28\9\2025</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>م.محمد عبدالله</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>918</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>1\11\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">تم سن فلاتس وعياره </t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">م.محمد عبدالله </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L14" t="inlineStr">
         <is>
           <t>2\2\2025</t>
@@ -10758,6 +10694,47 @@
       <c r="O14" t="inlineStr">
         <is>
           <t>م.عبدالله</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>5/11/2025</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>قطع سير900</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>تم تغير سير</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>مصطفي</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card24 by admin at 2025-12-01 06:52:18
</commit_message>
<xml_diff>
--- a/elquds.xlsx
+++ b/elquds.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,26 +561,66 @@
           <t>.1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
           <t>تم التشغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O2" t="inlineStr">
         <is>
           <t>م.صيام</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -598,19 +638,71 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -628,19 +720,71 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -658,19 +802,71 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -693,7 +889,11 @@
           <t>632</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -714,17 +914,41 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -747,7 +971,11 @@
           <t>870</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -758,19 +986,51 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>6\10\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -788,19 +1048,71 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -818,19 +1130,71 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -848,19 +1212,71 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -878,19 +1294,71 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -908,19 +1376,71 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -928,16 +1448,56 @@
           <t>24</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L13" t="inlineStr">
         <is>
           <t>12\11\2024</t>
@@ -953,8 +1513,16 @@
           <t>اعاده عيار</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -962,20 +1530,56 @@
           <t>24</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>800</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L14" t="inlineStr">
         <is>
           <t>11\2\2025</t>
@@ -991,8 +1595,58 @@
           <t>تم تغير زيت</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>950</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>1/12/2025</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>قطع سير كويلر 1270</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>تم تغير سير كويلر 1270</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>مصطفي</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9611,7 +10265,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9712,61 +10366,21 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
           <t>تم الشتغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>A.Elshenawy</t>
@@ -9789,11 +10403,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -9804,51 +10414,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>16\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -9866,11 +10444,7 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>✔</t>
@@ -9886,46 +10460,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
           <t>27\2\2025</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -9943,66 +10489,18 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -10025,61 +10523,25 @@
           <t>559</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>7\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -10102,36 +10564,16 @@
           <t>727</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10142,21 +10584,9 @@
           <t>6\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -10179,11 +10609,7 @@
           <t>860</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10194,41 +10620,17 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>28\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
           <t>م.محمد عبدالله</t>
@@ -10261,36 +10663,12 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
           <t>1\11\2025</t>
@@ -10301,11 +10679,7 @@
           <t xml:space="preserve">تم سن فلاتس وعياره </t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
           <t xml:space="preserve">م.محمد عبدالله </t>
@@ -10328,66 +10702,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -10405,66 +10731,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -10482,66 +10760,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -10559,66 +10789,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -10626,56 +10808,20 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
           <t>99</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
           <t>2\2\2025</t>
@@ -10694,47 +10840,6 @@
       <c r="O14" t="inlineStr">
         <is>
           <t>م.عبدالله</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>5/11/2025</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>قطع سير900</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>تم تغير سير</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>مصطفي</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card24 by admin at 2025-12-02 10:27:10
</commit_message>
<xml_diff>
--- a/elquds.xlsx
+++ b/elquds.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1612,20 +1612,56 @@
           <t>24</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>950</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L15" t="inlineStr">
         <is>
           <t>1/12/2025</t>
@@ -1646,7 +1682,53 @@
           <t>مصطفي</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr"/>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>968</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>زياره توكيل</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>تم  سن دوغر وسلندر وفلاتس وعيار ماكينه</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>خبير ارول</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card5 by admin at 2025-12-03 11:48:05
</commit_message>
<xml_diff>
--- a/elquds.xlsx
+++ b/elquds.xlsx
@@ -561,66 +561,26 @@
           <t>.1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
           <t>تم التشغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>م.صيام</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -638,71 +598,19 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -720,71 +628,19 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -802,71 +658,19 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -889,11 +693,7 @@
           <t>632</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -914,41 +714,17 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -971,11 +747,7 @@
           <t>870</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -986,51 +758,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>6\10\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1048,71 +788,19 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1130,71 +818,19 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1212,71 +848,19 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1294,71 +878,19 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1376,71 +908,19 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1448,56 +928,16 @@
           <t>24</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
           <t>12\11\2024</t>
@@ -1513,16 +953,8 @@
           <t>اعاده عيار</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1530,56 +962,20 @@
           <t>24</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
           <t>800</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
           <t>11\2\2025</t>
@@ -1595,16 +991,8 @@
           <t>تم تغير زيت</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1612,56 +1000,20 @@
           <t>24</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
           <t>950</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
           <t>1/12/2025</t>
@@ -1682,11 +1034,7 @@
           <t>مصطفي</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="P15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -7404,7 +6752,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7505,18 +6853,66 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7549,19 +6945,51 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>21\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7579,18 +7007,66 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7608,7 +7084,11 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7624,22 +7104,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>27\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7662,25 +7166,61 @@
           <t>566</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>10\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7703,16 +7243,36 @@
           <t>737</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7723,9 +7283,21 @@
           <t>16\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7753,12 +7325,36 @@
           <t>✅</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>23/11/2025</t>
@@ -7769,7 +7365,11 @@
           <t>تم سن الفلاتس</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O8" t="inlineStr">
         <is>
           <t xml:space="preserve">م.محمد عبدالله </t>
@@ -7797,7 +7397,11 @@
           <t>851</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7808,18 +7412,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L9" t="inlineStr">
         <is>
           <t>22\9\2025</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7837,18 +7469,66 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -7866,18 +7546,66 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -7895,18 +7623,66 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -7924,18 +7700,107 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2\12\2025</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>تم تغير</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>قطع سي1270</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>محمود</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>